<commit_message>
uploading the tableau file
</commit_message>
<xml_diff>
--- a/Entertainer analysis data raw.xlsx
+++ b/Entertainer analysis data raw.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neham\git practice\entertainer-data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48AC34B-4D82-4A92-93FD-6085AACE62E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BBE9AE-1DBF-441B-B462-FF4657996225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{105220EA-36A2-4F00-8F49-05004CCCCF60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$71</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -816,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1ACF7B6-9CB3-479B-928C-6A6F1BC0D49B}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2546,6 +2549,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H71" xr:uid="{E1ACF7B6-9CB3-479B-928C-6A6F1BC0D49B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>